<commit_message>
Fixed some issues with Excel documents.
Fixed lack of auto_increment in SQL setup script.
</commit_message>
<xml_diff>
--- a/ExcelTemplates/FutureShopTemplate-Valid.xlsx
+++ b/ExcelTemplates/FutureShopTemplate-Valid.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Seller</t>
   </si>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,75 +621,91 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated and working FutureShop template
</commit_message>
<xml_diff>
--- a/ExcelTemplates/FutureShopTemplate-Valid.xlsx
+++ b/ExcelTemplates/FutureShopTemplate-Valid.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Seller</t>
   </si>
@@ -67,9 +67,6 @@
     <t>SearchURL</t>
   </si>
   <si>
-    <t>http://www.futureshop.ca/Search/SearchResults.aspx</t>
-  </si>
-  <si>
     <t>SearchURL_PageParameter</t>
   </si>
   <si>
@@ -116,6 +113,21 @@
   </si>
   <si>
     <t>Item_Attribute_Name</t>
+  </si>
+  <si>
+    <t>span</t>
+  </si>
+  <si>
+    <t>dollars</t>
+  </si>
+  <si>
+    <t>h4</t>
+  </si>
+  <si>
+    <t>prod-title</t>
+  </si>
+  <si>
+    <t>http://www.futureshop.ca/Search/SearchResults.aspx?</t>
   </si>
   <si>
     <t>content_location</t>
@@ -125,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +158,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,13 +184,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -496,9 +519,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -520,132 +543,135 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
         <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,65 +679,129 @@
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>